<commit_message>
second commit change for create audio trigger
</commit_message>
<xml_diff>
--- a/file/data.xlsx
+++ b/file/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10335" activeTab="4"/>
+    <workbookView windowWidth="22943" windowHeight="9875" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>uname</t>
   </si>
@@ -65,7 +65,7 @@
     <t>Offer</t>
   </si>
   <si>
-    <t>Check</t>
+    <t>Papa John's</t>
   </si>
   <si>
     <t>Message</t>
@@ -83,10 +83,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>Automation_Campaign36</t>
-  </si>
-  <si>
-    <t>Automation_Campaign33</t>
+    <t>Automation_CampaignOct1</t>
   </si>
   <si>
     <t>trigger_name</t>
@@ -120,10 +117,10 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Storycard4</t>
-  </si>
-  <si>
-    <t>TestCard4</t>
+    <t>Storycardoct1</t>
+  </si>
+  <si>
+    <t>octcard1</t>
   </si>
   <si>
     <t>http://www.test.com</t>
@@ -144,9 +141,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -178,6 +175,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -185,15 +197,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,18 +211,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -239,15 +251,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,28 +267,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -292,22 +304,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,13 +319,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,169 +499,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,6 +510,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,15 +569,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -556,36 +583,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,7 +613,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -634,128 +631,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1098,9 +1095,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="19.552380952381" customWidth="1"/>
+    <col min="1" max="1" width="19.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1131,18 +1128,19 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="10.5714285714286" customWidth="1"/>
-    <col min="2" max="3" width="6.85714285714286" customWidth="1"/>
-    <col min="4" max="4" width="9.28571428571429" customWidth="1"/>
-    <col min="5" max="6" width="10.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="14.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="12.1428571428571" customWidth="1"/>
-    <col min="9" max="10" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="10.5740740740741" customWidth="1"/>
+    <col min="2" max="2" width="6.86111111111111" customWidth="1"/>
+    <col min="3" max="3" width="11.2222222222222" customWidth="1"/>
+    <col min="4" max="4" width="9.28703703703704" customWidth="1"/>
+    <col min="5" max="6" width="10.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="14.712962962963" customWidth="1"/>
+    <col min="8" max="8" width="12.1388888888889" customWidth="1"/>
+    <col min="9" max="10" width="13.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1179,7 +1177,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="3">
-        <v>6387</v>
+        <v>12404</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1222,13 +1220,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="23.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="11.4285714285714"/>
+    <col min="1" max="2" width="23.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="11.4259259259259"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1244,7 +1242,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1262,31 +1260,31 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16" customHeight="1" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="16" customHeight="1" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
@@ -1304,17 +1302,17 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="11.5740740740741" customWidth="1"/>
+    <col min="3" max="3" width="21.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="10.5740740740741" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="13.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="13.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1322,39 +1320,39 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code for Add user and Add Beacon pages
</commit_message>
<xml_diff>
--- a/file/data.xlsx
+++ b/file/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9875" activeTab="4"/>
+    <workbookView windowWidth="22943" windowHeight="9875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="createcampaign" sheetId="3" r:id="rId3"/>
     <sheet name="searchTrigger" sheetId="4" r:id="rId4"/>
     <sheet name="createcard" sheetId="5" r:id="rId5"/>
+    <sheet name="adduser" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>uname</t>
   </si>
@@ -133,6 +134,36 @@
   </si>
   <si>
     <t>click-through</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>ddd@abc.com</t>
+  </si>
+  <si>
+    <t>ACTV8 CMS Dashboard</t>
+  </si>
+  <si>
+    <t>Superadmin</t>
   </si>
 </sst>
 </file>
@@ -140,15 +171,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -166,38 +205,22 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,6 +234,89 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -221,90 +327,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,13 +350,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,169 +524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,21 +541,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -567,26 +583,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -605,23 +601,58 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -631,145 +662,145 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,7 +1140,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1176,7 +1207,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>12404</v>
       </c>
       <c r="B2" t="s">
@@ -1197,13 +1228,13 @@
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="5">
         <v>43300</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>43321</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="6">
         <v>43326</v>
       </c>
     </row>
@@ -1277,7 +1308,7 @@
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
@@ -1288,7 +1319,7 @@
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:1">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -1301,7 +1332,7 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1359,4 +1390,77 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="10.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="10.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="13.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="21.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="11.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ddd@abc.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>